<commit_message>
Computed duration matrix, shortest TSP paths from each node
</commit_message>
<xml_diff>
--- a/Documents/input.xlsx
+++ b/Documents/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/rodev_cisco_com/Documents/Documents/Github/Procomm_Scheduler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/rodev_cisco_com/Documents/Documents/Github/Procomm_Scheduler/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC104858111F72645ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9F424F-9E30-4AD4-89D2-0CE440E570A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPANIES" sheetId="1" r:id="rId1"/>
@@ -386,17 +386,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>120359</v>
       </c>
@@ -412,7 +410,7 @@
         <v>667970</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>120462</v>
       </c>
@@ -420,7 +418,7 @@
         <v>679910</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>120379</v>
       </c>
@@ -428,7 +426,7 @@
         <v>618495</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>120343</v>
       </c>
@@ -436,12 +434,12 @@
         <v>641682</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>120332</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>120429</v>
       </c>
@@ -460,32 +458,32 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>

</xml_diff>